<commit_message>
updating with data analysis and data clean up
</commit_message>
<xml_diff>
--- a/data_extraction/additional_data/baselines/NST-EST2024-POP.xlsx
+++ b/data_extraction/additional_data/baselines/NST-EST2024-POP.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamelder/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaitlinsinger/wa_notify/DEN_future/data_extraction/additional_data/baselines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29889941-97F1-1643-A6BB-FB6D44617814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CC50BB-7630-E249-917E-20F37164067E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20000" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4040" yWindow="500" windowWidth="20000" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NST-EST2024-POP" sheetId="1" r:id="rId1"/>
+    <sheet name="clean" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_NST01">'NST-EST2024-POP'!$A$4:$G$62</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
   <si>
     <t>United States</t>
   </si>
@@ -750,6 +751,21 @@
   </si>
   <si>
     <t>The Census Bureau has reviewed this data product to ensure appropriate access, use, and disclosure avoidance protection of the confidential source data used to produce this product (Data Management System (DMS) number:  P-6000042 and P-7501659. Disclosure Review Board (DRB) approval number: CBDRB-FY25-0078).</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>2021_pop</t>
+  </si>
+  <si>
+    <t>2020_pop</t>
+  </si>
+  <si>
+    <t>2022_pop</t>
+  </si>
+  <si>
+    <t>2023_pop</t>
   </si>
 </sst>
 </file>
@@ -1145,32 +1161,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -1213,6 +1203,32 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1520,8 +1536,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -1532,41 +1548,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="2.25" customHeight="1">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:36" ht="30.75" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:36" s="12" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -1598,8 +1614,8 @@
       <c r="AJ3" s="17"/>
     </row>
     <row r="4" spans="1:36" s="2" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="3">
         <v>2020</v>
       </c>
@@ -2937,84 +2953,84 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="27" customHeight="1">
-      <c r="A63" s="30" t="s">
+      <c r="A63" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="32"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="20"/>
     </row>
     <row r="64" spans="1:7" ht="48" customHeight="1">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="19"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="20"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="31"/>
     </row>
     <row r="65" spans="1:7">
-      <c r="A65" s="21" t="s">
+      <c r="A65" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="22"/>
-      <c r="D65" s="22"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="23"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="34"/>
     </row>
     <row r="66" spans="1:7" ht="27.75" customHeight="1">
-      <c r="A66" s="24" t="s">
+      <c r="A66" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
-      <c r="G66" s="26"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="37"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="24" t="s">
+      <c r="A67" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="26"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="37"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="27" t="s">
+      <c r="A68" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B68" s="28"/>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="29"/>
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="A68:G68"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:G3"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="A68:G68"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="80" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -3023,4 +3039,903 @@
     <brk id="6" max="1048575" man="1"/>
   </colBreaks>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4386BED2-D857-614A-B84F-E58F206917C7}">
+  <dimension ref="A1:E52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7">
+        <v>5033094</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5049196</v>
+      </c>
+      <c r="D2" s="7">
+        <v>5076181</v>
+      </c>
+      <c r="E2" s="7">
+        <v>5117673</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7">
+        <v>733017</v>
+      </c>
+      <c r="C3" s="7">
+        <v>734420</v>
+      </c>
+      <c r="D3" s="7">
+        <v>734442</v>
+      </c>
+      <c r="E3" s="7">
+        <v>736510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7">
+        <v>7187135</v>
+      </c>
+      <c r="C4" s="7">
+        <v>7274078</v>
+      </c>
+      <c r="D4" s="7">
+        <v>7377566</v>
+      </c>
+      <c r="E4" s="7">
+        <v>7473027</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3014546</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3026870</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3047704</v>
+      </c>
+      <c r="E5" s="7">
+        <v>3069463</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="7">
+        <v>39521958</v>
+      </c>
+      <c r="C6" s="7">
+        <v>39142565</v>
+      </c>
+      <c r="D6" s="7">
+        <v>39142414</v>
+      </c>
+      <c r="E6" s="7">
+        <v>39198693</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7">
+        <v>5787129</v>
+      </c>
+      <c r="C7" s="7">
+        <v>5814036</v>
+      </c>
+      <c r="D7" s="7">
+        <v>5850935</v>
+      </c>
+      <c r="E7" s="7">
+        <v>5901339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7">
+        <v>3579918</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3606607</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3617925</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3643023</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7">
+        <v>991928</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1005062</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1020625</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1036423</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="7">
+        <v>670917</v>
+      </c>
+      <c r="C10" s="7">
+        <v>669256</v>
+      </c>
+      <c r="D10" s="7">
+        <v>676725</v>
+      </c>
+      <c r="E10" s="7">
+        <v>687324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7">
+        <v>21592035</v>
+      </c>
+      <c r="C11" s="7">
+        <v>21831949</v>
+      </c>
+      <c r="D11" s="7">
+        <v>22379312</v>
+      </c>
+      <c r="E11" s="7">
+        <v>22904868</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="7">
+        <v>10732888</v>
+      </c>
+      <c r="C12" s="7">
+        <v>10792060</v>
+      </c>
+      <c r="D12" s="7">
+        <v>10931805</v>
+      </c>
+      <c r="E12" s="7">
+        <v>11064432</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1451252</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1447029</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1440359</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1441387</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1849415</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1904848</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1944299</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1971122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="7">
+        <v>12799088</v>
+      </c>
+      <c r="C15" s="7">
+        <v>12700641</v>
+      </c>
+      <c r="D15" s="7">
+        <v>12621821</v>
+      </c>
+      <c r="E15" s="7">
+        <v>12642259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="7">
+        <v>6790497</v>
+      </c>
+      <c r="C16" s="7">
+        <v>6815907</v>
+      </c>
+      <c r="D16" s="7">
+        <v>6844545</v>
+      </c>
+      <c r="E16" s="7">
+        <v>6880131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3191141</v>
+      </c>
+      <c r="C17" s="7">
+        <v>3198613</v>
+      </c>
+      <c r="D17" s="7">
+        <v>3202820</v>
+      </c>
+      <c r="E17" s="7">
+        <v>3218414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2938172</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2938338</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2937324</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2951500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="7">
+        <v>4508318</v>
+      </c>
+      <c r="C19" s="7">
+        <v>4507583</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4519233</v>
+      </c>
+      <c r="E19" s="7">
+        <v>4550595</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="7">
+        <v>4652301</v>
+      </c>
+      <c r="C20" s="7">
+        <v>4627971</v>
+      </c>
+      <c r="D20" s="7">
+        <v>4593687</v>
+      </c>
+      <c r="E20" s="7">
+        <v>4588071</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1364571</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1378931</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1390922</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1399646</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="7">
+        <v>6177935</v>
+      </c>
+      <c r="C22" s="7">
+        <v>6179403</v>
+      </c>
+      <c r="D22" s="7">
+        <v>6192440</v>
+      </c>
+      <c r="E22" s="7">
+        <v>6217062</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="7">
+        <v>6994598</v>
+      </c>
+      <c r="C23" s="7">
+        <v>7000474</v>
+      </c>
+      <c r="D23" s="7">
+        <v>7022468</v>
+      </c>
+      <c r="E23" s="7">
+        <v>7066568</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="7">
+        <v>10072703</v>
+      </c>
+      <c r="C24" s="7">
+        <v>10041351</v>
+      </c>
+      <c r="D24" s="7">
+        <v>10050877</v>
+      </c>
+      <c r="E24" s="7">
+        <v>10083356</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="7">
+        <v>5710735</v>
+      </c>
+      <c r="C25" s="7">
+        <v>5718660</v>
+      </c>
+      <c r="D25" s="7">
+        <v>5721621</v>
+      </c>
+      <c r="E25" s="7">
+        <v>5753048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2958536</v>
+      </c>
+      <c r="C26" s="7">
+        <v>2947209</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2941939</v>
+      </c>
+      <c r="E26" s="7">
+        <v>2943172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="7">
+        <v>6154744</v>
+      </c>
+      <c r="C27" s="7">
+        <v>6171374</v>
+      </c>
+      <c r="D27" s="7">
+        <v>6179414</v>
+      </c>
+      <c r="E27" s="7">
+        <v>6208038</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1087230</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1106522</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1122095</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1131302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1963387</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1964537</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1972246</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1987864</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="7">
+        <v>3116967</v>
+      </c>
+      <c r="C30" s="7">
+        <v>3148141</v>
+      </c>
+      <c r="D30" s="7">
+        <v>3176116</v>
+      </c>
+      <c r="E30" s="7">
+        <v>3214363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="7">
+        <v>1378756</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1387677</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1396678</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1402199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="7">
+        <v>9272794</v>
+      </c>
+      <c r="C32" s="7">
+        <v>9270541</v>
+      </c>
+      <c r="D32" s="7">
+        <v>9295227</v>
+      </c>
+      <c r="E32" s="7">
+        <v>9379642</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="7">
+        <v>2118606</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2117333</v>
+      </c>
+      <c r="D33" s="7">
+        <v>2113868</v>
+      </c>
+      <c r="E33" s="7">
+        <v>2121164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="7">
+        <v>20105171</v>
+      </c>
+      <c r="C34" s="7">
+        <v>19848276</v>
+      </c>
+      <c r="D34" s="7">
+        <v>19703747</v>
+      </c>
+      <c r="E34" s="7">
+        <v>19737367</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="7">
+        <v>10449652</v>
+      </c>
+      <c r="C35" s="7">
+        <v>10564320</v>
+      </c>
+      <c r="D35" s="7">
+        <v>10710793</v>
+      </c>
+      <c r="E35" s="7">
+        <v>10881189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="7">
+        <v>779563</v>
+      </c>
+      <c r="C36" s="7">
+        <v>777966</v>
+      </c>
+      <c r="D36" s="7">
+        <v>781057</v>
+      </c>
+      <c r="E36" s="7">
+        <v>789047</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="7">
+        <v>11798905</v>
+      </c>
+      <c r="C37" s="7">
+        <v>11767344</v>
+      </c>
+      <c r="D37" s="7">
+        <v>11777874</v>
+      </c>
+      <c r="E37" s="7">
+        <v>11824034</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="7">
+        <v>3965415</v>
+      </c>
+      <c r="C38" s="7">
+        <v>3992238</v>
+      </c>
+      <c r="D38" s="7">
+        <v>4026229</v>
+      </c>
+      <c r="E38" s="7">
+        <v>4063882</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="7">
+        <v>4243779</v>
+      </c>
+      <c r="C39" s="7">
+        <v>4254280</v>
+      </c>
+      <c r="D39" s="7">
+        <v>4247372</v>
+      </c>
+      <c r="E39" s="7">
+        <v>4253653</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="7">
+        <v>12996143</v>
+      </c>
+      <c r="C40" s="7">
+        <v>13015571</v>
+      </c>
+      <c r="D40" s="7">
+        <v>12984990</v>
+      </c>
+      <c r="E40" s="7">
+        <v>13017721</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1096530</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1097246</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1099498</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1103429</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" s="7">
+        <v>5132249</v>
+      </c>
+      <c r="C42" s="7">
+        <v>5194274</v>
+      </c>
+      <c r="D42" s="7">
+        <v>5287935</v>
+      </c>
+      <c r="E42" s="7">
+        <v>5387830</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="7">
+        <v>887948</v>
+      </c>
+      <c r="C43" s="7">
+        <v>896492</v>
+      </c>
+      <c r="D43" s="7">
+        <v>909723</v>
+      </c>
+      <c r="E43" s="7">
+        <v>918305</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" s="7">
+        <v>6927904</v>
+      </c>
+      <c r="C44" s="7">
+        <v>6965740</v>
+      </c>
+      <c r="D44" s="7">
+        <v>7062217</v>
+      </c>
+      <c r="E44" s="7">
+        <v>7148304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="7">
+        <v>29239570</v>
+      </c>
+      <c r="C45" s="7">
+        <v>29570351</v>
+      </c>
+      <c r="D45" s="7">
+        <v>30113488</v>
+      </c>
+      <c r="E45" s="7">
+        <v>30727890</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="7">
+        <v>3284077</v>
+      </c>
+      <c r="C46" s="7">
+        <v>3339738</v>
+      </c>
+      <c r="D46" s="7">
+        <v>3391011</v>
+      </c>
+      <c r="E46" s="7">
+        <v>3443222</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="7">
+        <v>642977</v>
+      </c>
+      <c r="C47" s="7">
+        <v>647210</v>
+      </c>
+      <c r="D47" s="7">
+        <v>648142</v>
+      </c>
+      <c r="E47" s="7">
+        <v>648708</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="7">
+        <v>8637615</v>
+      </c>
+      <c r="C48" s="7">
+        <v>8658910</v>
+      </c>
+      <c r="D48" s="7">
+        <v>8683414</v>
+      </c>
+      <c r="E48" s="7">
+        <v>8734685</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="7">
+        <v>7727209</v>
+      </c>
+      <c r="C49" s="7">
+        <v>7743760</v>
+      </c>
+      <c r="D49" s="7">
+        <v>7794123</v>
+      </c>
+      <c r="E49" s="7">
+        <v>7857320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="7">
+        <v>1791646</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1785618</v>
+      </c>
+      <c r="D50" s="7">
+        <v>1774122</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1770495</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="7">
+        <v>5897375</v>
+      </c>
+      <c r="C51" s="7">
+        <v>5881608</v>
+      </c>
+      <c r="D51" s="7">
+        <v>5903975</v>
+      </c>
+      <c r="E51" s="7">
+        <v>5930405</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="7">
+        <v>577681</v>
+      </c>
+      <c r="C52" s="7">
+        <v>579636</v>
+      </c>
+      <c r="D52" s="7">
+        <v>581978</v>
+      </c>
+      <c r="E52" s="7">
+        <v>585067</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>